<commit_message>
update data for OPM for 2023 and 2024
</commit_message>
<xml_diff>
--- a/data/Oficina_de_procuradora_de_mujeres/opmPartMes.xlsx
+++ b/data/Oficina_de_procuradora_de_mujeres/opmPartMes.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29103"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariana.pagan\Desktop\Comite PARE\OPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlando.hernandez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E11AC43-ADBE-49AF-ADDF-ECA84175DBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24270" windowHeight="10830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="mensual" sheetId="2" r:id="rId1"/>
+    <sheet name="anual" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,12 +37,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="11">
   <si>
     <t>month</t>
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>cantidad</t>
   </si>
   <si>
     <t>Violencia doméstica (VD)</t>
@@ -60,17 +69,14 @@
     <t>Otras</t>
   </si>
   <si>
-    <t>tipo</t>
-  </si>
-  <si>
-    <t>cantidad</t>
+    <t>Trata Humana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,19 +420,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F213" sqref="F213"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,13 +440,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -448,13 +454,13 @@
         <v>2020</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -462,13 +468,13 @@
         <v>2020</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -476,13 +482,13 @@
         <v>2020</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -490,13 +496,13 @@
         <v>2020</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -504,13 +510,13 @@
         <v>2020</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -518,13 +524,13 @@
         <v>2020</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -532,13 +538,13 @@
         <v>2020</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -546,13 +552,13 @@
         <v>2020</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -560,13 +566,13 @@
         <v>2020</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -574,13 +580,13 @@
         <v>2020</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -588,13 +594,13 @@
         <v>2020</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -602,13 +608,13 @@
         <v>2020</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -616,13 +622,13 @@
         <v>2021</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -630,13 +636,13 @@
         <v>2021</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>3</v>
       </c>
@@ -644,13 +650,13 @@
         <v>2021</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>4</v>
       </c>
@@ -658,13 +664,13 @@
         <v>2021</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>5</v>
       </c>
@@ -672,13 +678,13 @@
         <v>2021</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>6</v>
       </c>
@@ -686,13 +692,13 @@
         <v>2021</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>7</v>
       </c>
@@ -700,13 +706,13 @@
         <v>2021</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>8</v>
       </c>
@@ -714,13 +720,13 @@
         <v>2021</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>9</v>
       </c>
@@ -728,13 +734,13 @@
         <v>2021</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>10</v>
       </c>
@@ -742,13 +748,13 @@
         <v>2021</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D23">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>11</v>
       </c>
@@ -756,13 +762,13 @@
         <v>2021</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D24">
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>12</v>
       </c>
@@ -770,13 +776,13 @@
         <v>2021</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D25">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>1</v>
       </c>
@@ -784,13 +790,13 @@
         <v>2022</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -798,13 +804,13 @@
         <v>2022</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>3</v>
       </c>
@@ -812,13 +818,13 @@
         <v>2022</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D28">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>4</v>
       </c>
@@ -826,13 +832,13 @@
         <v>2022</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D29">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>5</v>
       </c>
@@ -840,13 +846,13 @@
         <v>2022</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D30">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>6</v>
       </c>
@@ -854,13 +860,13 @@
         <v>2022</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D31">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>7</v>
       </c>
@@ -868,13 +874,13 @@
         <v>2022</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D32">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>8</v>
       </c>
@@ -882,13 +888,13 @@
         <v>2022</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D33">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>9</v>
       </c>
@@ -896,13 +902,13 @@
         <v>2022</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D34">
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>10</v>
       </c>
@@ -910,13 +916,13 @@
         <v>2022</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D35">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>11</v>
       </c>
@@ -924,13 +930,13 @@
         <v>2022</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D36">
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>12</v>
       </c>
@@ -938,13 +944,13 @@
         <v>2022</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D37">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>1</v>
       </c>
@@ -952,13 +958,13 @@
         <v>2020</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D38">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>2</v>
       </c>
@@ -966,13 +972,13 @@
         <v>2020</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D39">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -980,13 +986,13 @@
         <v>2020</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D40">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>4</v>
       </c>
@@ -994,13 +1000,13 @@
         <v>2020</v>
       </c>
       <c r="C41" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1008,13 +1014,13 @@
         <v>2020</v>
       </c>
       <c r="C42" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>6</v>
       </c>
@@ -1022,13 +1028,13 @@
         <v>2020</v>
       </c>
       <c r="C43" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>7</v>
       </c>
@@ -1036,13 +1042,13 @@
         <v>2020</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D44">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>8</v>
       </c>
@@ -1050,13 +1056,13 @@
         <v>2020</v>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>9</v>
       </c>
@@ -1064,13 +1070,13 @@
         <v>2020</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D46">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>10</v>
       </c>
@@ -1078,13 +1084,13 @@
         <v>2020</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D47">
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>11</v>
       </c>
@@ -1092,13 +1098,13 @@
         <v>2020</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D48">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>12</v>
       </c>
@@ -1106,13 +1112,13 @@
         <v>2020</v>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D49">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>1</v>
       </c>
@@ -1120,13 +1126,13 @@
         <v>2021</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D50">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>2</v>
       </c>
@@ -1134,13 +1140,13 @@
         <v>2021</v>
       </c>
       <c r="C51" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D51">
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -1148,13 +1154,13 @@
         <v>2021</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D52">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>4</v>
       </c>
@@ -1162,13 +1168,13 @@
         <v>2021</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D53">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>5</v>
       </c>
@@ -1176,13 +1182,13 @@
         <v>2021</v>
       </c>
       <c r="C54" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D54">
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>6</v>
       </c>
@@ -1190,13 +1196,13 @@
         <v>2021</v>
       </c>
       <c r="C55" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D55">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>7</v>
       </c>
@@ -1204,13 +1210,13 @@
         <v>2021</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D56">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>8</v>
       </c>
@@ -1218,13 +1224,13 @@
         <v>2021</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D57">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>9</v>
       </c>
@@ -1232,13 +1238,13 @@
         <v>2021</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D58">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>10</v>
       </c>
@@ -1246,13 +1252,13 @@
         <v>2021</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D59">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>11</v>
       </c>
@@ -1260,13 +1266,13 @@
         <v>2021</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D60">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>12</v>
       </c>
@@ -1274,13 +1280,13 @@
         <v>2021</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D61">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>1</v>
       </c>
@@ -1288,13 +1294,13 @@
         <v>2022</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D62">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>2</v>
       </c>
@@ -1302,13 +1308,13 @@
         <v>2022</v>
       </c>
       <c r="C63" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D63">
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>3</v>
       </c>
@@ -1316,13 +1322,13 @@
         <v>2022</v>
       </c>
       <c r="C64" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D64">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>4</v>
       </c>
@@ -1330,13 +1336,13 @@
         <v>2022</v>
       </c>
       <c r="C65" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D65">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>5</v>
       </c>
@@ -1344,13 +1350,13 @@
         <v>2022</v>
       </c>
       <c r="C66" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D66">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>6</v>
       </c>
@@ -1358,13 +1364,13 @@
         <v>2022</v>
       </c>
       <c r="C67" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D67">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>7</v>
       </c>
@@ -1372,13 +1378,13 @@
         <v>2022</v>
       </c>
       <c r="C68" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D68">
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>8</v>
       </c>
@@ -1386,13 +1392,13 @@
         <v>2022</v>
       </c>
       <c r="C69" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D69">
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>9</v>
       </c>
@@ -1400,13 +1406,13 @@
         <v>2022</v>
       </c>
       <c r="C70" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D70">
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>10</v>
       </c>
@@ -1414,13 +1420,13 @@
         <v>2022</v>
       </c>
       <c r="C71" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D71">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>11</v>
       </c>
@@ -1428,13 +1434,13 @@
         <v>2022</v>
       </c>
       <c r="C72" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D72">
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>12</v>
       </c>
@@ -1442,13 +1448,13 @@
         <v>2022</v>
       </c>
       <c r="C73" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D73">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>1</v>
       </c>
@@ -1456,13 +1462,13 @@
         <v>2020</v>
       </c>
       <c r="C74" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>2</v>
       </c>
@@ -1470,13 +1476,13 @@
         <v>2020</v>
       </c>
       <c r="C75" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D75">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>3</v>
       </c>
@@ -1484,13 +1490,13 @@
         <v>2020</v>
       </c>
       <c r="C76" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D76">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>4</v>
       </c>
@@ -1498,13 +1504,13 @@
         <v>2020</v>
       </c>
       <c r="C77" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>5</v>
       </c>
@@ -1512,13 +1518,13 @@
         <v>2020</v>
       </c>
       <c r="C78" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D78">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>6</v>
       </c>
@@ -1526,13 +1532,13 @@
         <v>2020</v>
       </c>
       <c r="C79" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>7</v>
       </c>
@@ -1540,13 +1546,13 @@
         <v>2020</v>
       </c>
       <c r="C80" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>8</v>
       </c>
@@ -1554,13 +1560,13 @@
         <v>2020</v>
       </c>
       <c r="C81" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>9</v>
       </c>
@@ -1568,13 +1574,13 @@
         <v>2020</v>
       </c>
       <c r="C82" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>10</v>
       </c>
@@ -1582,13 +1588,13 @@
         <v>2020</v>
       </c>
       <c r="C83" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D83">
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>11</v>
       </c>
@@ -1596,13 +1602,13 @@
         <v>2020</v>
       </c>
       <c r="C84" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D84">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>12</v>
       </c>
@@ -1610,13 +1616,13 @@
         <v>2020</v>
       </c>
       <c r="C85" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D85">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>1</v>
       </c>
@@ -1624,13 +1630,13 @@
         <v>2021</v>
       </c>
       <c r="C86" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D86">
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>2</v>
       </c>
@@ -1638,13 +1644,13 @@
         <v>2021</v>
       </c>
       <c r="C87" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D87">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>3</v>
       </c>
@@ -1652,13 +1658,13 @@
         <v>2021</v>
       </c>
       <c r="C88" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D88">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>4</v>
       </c>
@@ -1666,13 +1672,13 @@
         <v>2021</v>
       </c>
       <c r="C89" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D89">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>5</v>
       </c>
@@ -1680,13 +1686,13 @@
         <v>2021</v>
       </c>
       <c r="C90" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D90">
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>6</v>
       </c>
@@ -1694,13 +1700,13 @@
         <v>2021</v>
       </c>
       <c r="C91" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D91">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>7</v>
       </c>
@@ -1708,13 +1714,13 @@
         <v>2021</v>
       </c>
       <c r="C92" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D92">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>8</v>
       </c>
@@ -1722,13 +1728,13 @@
         <v>2021</v>
       </c>
       <c r="C93" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D93">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>9</v>
       </c>
@@ -1736,13 +1742,13 @@
         <v>2021</v>
       </c>
       <c r="C94" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D94">
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>10</v>
       </c>
@@ -1750,13 +1756,13 @@
         <v>2021</v>
       </c>
       <c r="C95" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D95">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>11</v>
       </c>
@@ -1764,13 +1770,13 @@
         <v>2021</v>
       </c>
       <c r="C96" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D96">
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>12</v>
       </c>
@@ -1778,13 +1784,13 @@
         <v>2021</v>
       </c>
       <c r="C97" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D97">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>1</v>
       </c>
@@ -1792,13 +1798,13 @@
         <v>2022</v>
       </c>
       <c r="C98" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D98">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>2</v>
       </c>
@@ -1806,13 +1812,13 @@
         <v>2022</v>
       </c>
       <c r="C99" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D99">
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>3</v>
       </c>
@@ -1820,13 +1826,13 @@
         <v>2022</v>
       </c>
       <c r="C100" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D100">
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>4</v>
       </c>
@@ -1834,13 +1840,13 @@
         <v>2022</v>
       </c>
       <c r="C101" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D101">
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102">
         <v>1</v>
       </c>
@@ -1848,13 +1854,13 @@
         <v>2020</v>
       </c>
       <c r="C102" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103">
         <v>2</v>
       </c>
@@ -1862,13 +1868,13 @@
         <v>2020</v>
       </c>
       <c r="C103" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104">
         <v>3</v>
       </c>
@@ -1876,13 +1882,13 @@
         <v>2020</v>
       </c>
       <c r="C104" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D104">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105">
         <v>4</v>
       </c>
@@ -1890,13 +1896,13 @@
         <v>2020</v>
       </c>
       <c r="C105" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D105">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106">
         <v>5</v>
       </c>
@@ -1904,13 +1910,13 @@
         <v>2020</v>
       </c>
       <c r="C106" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D106">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107">
         <v>6</v>
       </c>
@@ -1918,13 +1924,13 @@
         <v>2020</v>
       </c>
       <c r="C107" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D107">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108">
         <v>7</v>
       </c>
@@ -1932,13 +1938,13 @@
         <v>2020</v>
       </c>
       <c r="C108" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D108">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109">
         <v>8</v>
       </c>
@@ -1946,13 +1952,13 @@
         <v>2020</v>
       </c>
       <c r="C109" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D109">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110">
         <v>9</v>
       </c>
@@ -1960,13 +1966,13 @@
         <v>2020</v>
       </c>
       <c r="C110" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D110">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111">
         <v>10</v>
       </c>
@@ -1974,13 +1980,13 @@
         <v>2020</v>
       </c>
       <c r="C111" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D111">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112">
         <v>11</v>
       </c>
@@ -1988,13 +1994,13 @@
         <v>2020</v>
       </c>
       <c r="C112" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D112">
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113">
         <v>12</v>
       </c>
@@ -2002,13 +2008,13 @@
         <v>2020</v>
       </c>
       <c r="C113" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D113">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114">
         <v>1</v>
       </c>
@@ -2016,13 +2022,13 @@
         <v>2021</v>
       </c>
       <c r="C114" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D114">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115">
         <v>2</v>
       </c>
@@ -2030,13 +2036,13 @@
         <v>2021</v>
       </c>
       <c r="C115" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D115">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116">
         <v>3</v>
       </c>
@@ -2044,13 +2050,13 @@
         <v>2021</v>
       </c>
       <c r="C116" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D116">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117">
         <v>4</v>
       </c>
@@ -2058,13 +2064,13 @@
         <v>2021</v>
       </c>
       <c r="C117" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D117">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118">
         <v>5</v>
       </c>
@@ -2072,13 +2078,13 @@
         <v>2021</v>
       </c>
       <c r="C118" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D118">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119">
         <v>6</v>
       </c>
@@ -2086,13 +2092,13 @@
         <v>2021</v>
       </c>
       <c r="C119" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D119">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120">
         <v>7</v>
       </c>
@@ -2100,13 +2106,13 @@
         <v>2021</v>
       </c>
       <c r="C120" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D120">
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121">
         <v>8</v>
       </c>
@@ -2114,13 +2120,13 @@
         <v>2021</v>
       </c>
       <c r="C121" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D121">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122">
         <v>9</v>
       </c>
@@ -2128,13 +2134,13 @@
         <v>2021</v>
       </c>
       <c r="C122" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D122">
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123">
         <v>10</v>
       </c>
@@ -2142,13 +2148,13 @@
         <v>2021</v>
       </c>
       <c r="C123" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D123">
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124">
         <v>11</v>
       </c>
@@ -2156,13 +2162,13 @@
         <v>2021</v>
       </c>
       <c r="C124" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D124">
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125">
         <v>12</v>
       </c>
@@ -2170,13 +2176,13 @@
         <v>2021</v>
       </c>
       <c r="C125" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D125">
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126">
         <v>1</v>
       </c>
@@ -2184,13 +2190,13 @@
         <v>2022</v>
       </c>
       <c r="C126" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D126">
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127">
         <v>2</v>
       </c>
@@ -2198,13 +2204,13 @@
         <v>2022</v>
       </c>
       <c r="C127" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D127">
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128">
         <v>3</v>
       </c>
@@ -2212,13 +2218,13 @@
         <v>2022</v>
       </c>
       <c r="C128" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D128">
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129">
         <v>4</v>
       </c>
@@ -2226,13 +2232,13 @@
         <v>2022</v>
       </c>
       <c r="C129" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D129">
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130">
         <v>5</v>
       </c>
@@ -2240,13 +2246,13 @@
         <v>2022</v>
       </c>
       <c r="C130" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D130">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131">
         <v>6</v>
       </c>
@@ -2254,13 +2260,13 @@
         <v>2022</v>
       </c>
       <c r="C131" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D131">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132">
         <v>7</v>
       </c>
@@ -2268,13 +2274,13 @@
         <v>2022</v>
       </c>
       <c r="C132" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D132">
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133">
         <v>8</v>
       </c>
@@ -2282,13 +2288,13 @@
         <v>2022</v>
       </c>
       <c r="C133" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D133">
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134">
         <v>9</v>
       </c>
@@ -2296,13 +2302,13 @@
         <v>2022</v>
       </c>
       <c r="C134" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D134">
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135">
         <v>10</v>
       </c>
@@ -2310,13 +2316,13 @@
         <v>2022</v>
       </c>
       <c r="C135" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D135">
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136">
         <v>11</v>
       </c>
@@ -2324,13 +2330,13 @@
         <v>2022</v>
       </c>
       <c r="C136" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D136">
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137">
         <v>12</v>
       </c>
@@ -2338,13 +2344,13 @@
         <v>2022</v>
       </c>
       <c r="C137" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D137">
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138">
         <v>1</v>
       </c>
@@ -2352,13 +2358,13 @@
         <v>2020</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D138">
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139">
         <v>2</v>
       </c>
@@ -2366,13 +2372,13 @@
         <v>2020</v>
       </c>
       <c r="C139" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D139">
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140">
         <v>3</v>
       </c>
@@ -2380,13 +2386,13 @@
         <v>2020</v>
       </c>
       <c r="C140" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D140">
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141">
         <v>4</v>
       </c>
@@ -2394,13 +2400,13 @@
         <v>2020</v>
       </c>
       <c r="C141" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D141">
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142">
         <v>5</v>
       </c>
@@ -2408,13 +2414,13 @@
         <v>2020</v>
       </c>
       <c r="C142" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D142">
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143">
         <v>6</v>
       </c>
@@ -2422,13 +2428,13 @@
         <v>2020</v>
       </c>
       <c r="C143" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D143">
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144">
         <v>7</v>
       </c>
@@ -2436,13 +2442,13 @@
         <v>2020</v>
       </c>
       <c r="C144" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D144">
         <v>8</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145">
         <v>8</v>
       </c>
@@ -2450,13 +2456,13 @@
         <v>2020</v>
       </c>
       <c r="C145" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D145">
         <v>8</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146">
         <v>9</v>
       </c>
@@ -2464,13 +2470,13 @@
         <v>2020</v>
       </c>
       <c r="C146" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D146">
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147">
         <v>10</v>
       </c>
@@ -2478,13 +2484,13 @@
         <v>2020</v>
       </c>
       <c r="C147" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D147">
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148">
         <v>11</v>
       </c>
@@ -2492,13 +2498,13 @@
         <v>2020</v>
       </c>
       <c r="C148" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D148">
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4">
       <c r="A149">
         <v>12</v>
       </c>
@@ -2506,13 +2512,13 @@
         <v>2020</v>
       </c>
       <c r="C149" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D149">
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4">
       <c r="A150">
         <v>1</v>
       </c>
@@ -2520,13 +2526,13 @@
         <v>2021</v>
       </c>
       <c r="C150" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D150">
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4">
       <c r="A151">
         <v>2</v>
       </c>
@@ -2534,13 +2540,13 @@
         <v>2021</v>
       </c>
       <c r="C151" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D151">
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4">
       <c r="A152">
         <v>3</v>
       </c>
@@ -2548,13 +2554,13 @@
         <v>2021</v>
       </c>
       <c r="C152" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D152">
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4">
       <c r="A153">
         <v>4</v>
       </c>
@@ -2562,13 +2568,13 @@
         <v>2021</v>
       </c>
       <c r="C153" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D153">
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154">
         <v>5</v>
       </c>
@@ -2576,13 +2582,13 @@
         <v>2021</v>
       </c>
       <c r="C154" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D154">
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155">
         <v>6</v>
       </c>
@@ -2590,13 +2596,13 @@
         <v>2021</v>
       </c>
       <c r="C155" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D155">
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156">
         <v>7</v>
       </c>
@@ -2604,13 +2610,13 @@
         <v>2021</v>
       </c>
       <c r="C156" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D156">
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157">
         <v>8</v>
       </c>
@@ -2618,13 +2624,13 @@
         <v>2021</v>
       </c>
       <c r="C157" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D157">
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158">
         <v>9</v>
       </c>
@@ -2632,13 +2638,13 @@
         <v>2021</v>
       </c>
       <c r="C158" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D158">
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159">
         <v>10</v>
       </c>
@@ -2646,13 +2652,13 @@
         <v>2021</v>
       </c>
       <c r="C159" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D159">
         <v>16</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160">
         <v>11</v>
       </c>
@@ -2660,13 +2666,13 @@
         <v>2021</v>
       </c>
       <c r="C160" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D160">
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4">
       <c r="A161">
         <v>12</v>
       </c>
@@ -2674,13 +2680,13 @@
         <v>2021</v>
       </c>
       <c r="C161" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D161">
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4">
       <c r="A162">
         <v>1</v>
       </c>
@@ -2688,13 +2694,13 @@
         <v>2022</v>
       </c>
       <c r="C162" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D162">
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4">
       <c r="A163">
         <v>2</v>
       </c>
@@ -2702,13 +2708,13 @@
         <v>2022</v>
       </c>
       <c r="C163" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D163">
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4">
       <c r="A164">
         <v>3</v>
       </c>
@@ -2716,13 +2722,13 @@
         <v>2022</v>
       </c>
       <c r="C164" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D164">
         <v>14</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4">
       <c r="A165">
         <v>4</v>
       </c>
@@ -2730,13 +2736,13 @@
         <v>2022</v>
       </c>
       <c r="C165" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D165">
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4">
       <c r="A166">
         <v>5</v>
       </c>
@@ -2744,13 +2750,13 @@
         <v>2022</v>
       </c>
       <c r="C166" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D166">
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4">
       <c r="A167">
         <v>6</v>
       </c>
@@ -2758,13 +2764,13 @@
         <v>2022</v>
       </c>
       <c r="C167" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D167">
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4">
       <c r="A168">
         <v>7</v>
       </c>
@@ -2772,13 +2778,13 @@
         <v>2022</v>
       </c>
       <c r="C168" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D168">
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4">
       <c r="A169">
         <v>8</v>
       </c>
@@ -2786,13 +2792,13 @@
         <v>2022</v>
       </c>
       <c r="C169" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D169">
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4">
       <c r="A170">
         <v>9</v>
       </c>
@@ -2800,13 +2806,13 @@
         <v>2022</v>
       </c>
       <c r="C170" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D170">
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4">
       <c r="A171">
         <v>10</v>
       </c>
@@ -2814,13 +2820,13 @@
         <v>2022</v>
       </c>
       <c r="C171" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D171">
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4">
       <c r="A172">
         <v>11</v>
       </c>
@@ -2828,13 +2834,13 @@
         <v>2022</v>
       </c>
       <c r="C172" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D172">
         <v>31</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4">
       <c r="A173">
         <v>12</v>
       </c>
@@ -2842,13 +2848,13 @@
         <v>2022</v>
       </c>
       <c r="C173" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D173">
         <v>11</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4">
       <c r="A174">
         <v>1</v>
       </c>
@@ -2856,13 +2862,13 @@
         <v>2020</v>
       </c>
       <c r="C174" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D174">
         <v>168</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4">
       <c r="A175">
         <v>2</v>
       </c>
@@ -2870,13 +2876,13 @@
         <v>2020</v>
       </c>
       <c r="C175" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D175">
         <v>210</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4">
       <c r="A176">
         <v>3</v>
       </c>
@@ -2884,13 +2890,13 @@
         <v>2020</v>
       </c>
       <c r="C176" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D176">
         <v>163</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4">
       <c r="A177">
         <v>4</v>
       </c>
@@ -2898,13 +2904,13 @@
         <v>2020</v>
       </c>
       <c r="C177" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D177">
         <v>231</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4">
       <c r="A178">
         <v>5</v>
       </c>
@@ -2912,13 +2918,13 @@
         <v>2020</v>
       </c>
       <c r="C178" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D178">
         <v>202</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4">
       <c r="A179">
         <v>6</v>
       </c>
@@ -2926,13 +2932,13 @@
         <v>2020</v>
       </c>
       <c r="C179" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D179">
         <v>180</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4">
       <c r="A180">
         <v>7</v>
       </c>
@@ -2940,13 +2946,13 @@
         <v>2020</v>
       </c>
       <c r="C180" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D180">
         <v>153</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4">
       <c r="A181">
         <v>8</v>
       </c>
@@ -2954,13 +2960,13 @@
         <v>2020</v>
       </c>
       <c r="C181" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D181">
         <v>143</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4">
       <c r="A182">
         <v>9</v>
       </c>
@@ -2968,13 +2974,13 @@
         <v>2020</v>
       </c>
       <c r="C182" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D182">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4">
       <c r="A183">
         <v>10</v>
       </c>
@@ -2982,13 +2988,13 @@
         <v>2020</v>
       </c>
       <c r="C183" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D183">
         <v>212</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4">
       <c r="A184">
         <v>11</v>
       </c>
@@ -2996,13 +3002,13 @@
         <v>2020</v>
       </c>
       <c r="C184" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D184">
         <v>140</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4">
       <c r="A185">
         <v>12</v>
       </c>
@@ -3010,13 +3016,13 @@
         <v>2020</v>
       </c>
       <c r="C185" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D185">
         <v>112</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4">
       <c r="A186">
         <v>1</v>
       </c>
@@ -3024,13 +3030,13 @@
         <v>2021</v>
       </c>
       <c r="C186" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D186">
         <v>165</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4">
       <c r="A187">
         <v>2</v>
       </c>
@@ -3038,13 +3044,13 @@
         <v>2021</v>
       </c>
       <c r="C187" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D187">
         <v>190</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4">
       <c r="A188">
         <v>3</v>
       </c>
@@ -3052,13 +3058,13 @@
         <v>2021</v>
       </c>
       <c r="C188" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D188">
         <v>227</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4">
       <c r="A189">
         <v>4</v>
       </c>
@@ -3066,13 +3072,13 @@
         <v>2021</v>
       </c>
       <c r="C189" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D189">
         <v>142</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4">
       <c r="A190">
         <v>5</v>
       </c>
@@ -3080,13 +3086,13 @@
         <v>2021</v>
       </c>
       <c r="C190" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D190">
         <v>243</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4">
       <c r="A191">
         <v>6</v>
       </c>
@@ -3094,13 +3100,13 @@
         <v>2021</v>
       </c>
       <c r="C191" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D191">
         <v>244</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4">
       <c r="A192">
         <v>7</v>
       </c>
@@ -3108,13 +3114,13 @@
         <v>2021</v>
       </c>
       <c r="C192" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D192">
         <v>195</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4">
       <c r="A193">
         <v>8</v>
       </c>
@@ -3122,13 +3128,13 @@
         <v>2021</v>
       </c>
       <c r="C193" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D193">
         <v>206</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4">
       <c r="A194">
         <v>9</v>
       </c>
@@ -3136,13 +3142,13 @@
         <v>2021</v>
       </c>
       <c r="C194" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D194">
         <v>242</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4">
       <c r="A195">
         <v>10</v>
       </c>
@@ -3150,13 +3156,13 @@
         <v>2021</v>
       </c>
       <c r="C195" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D195">
         <v>234</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4">
       <c r="A196">
         <v>11</v>
       </c>
@@ -3164,13 +3170,13 @@
         <v>2021</v>
       </c>
       <c r="C196" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D196">
         <v>274</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4">
       <c r="A197">
         <v>12</v>
       </c>
@@ -3178,13 +3184,13 @@
         <v>2021</v>
       </c>
       <c r="C197" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D197">
         <v>252</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4">
       <c r="A198">
         <v>1</v>
       </c>
@@ -3192,13 +3198,13 @@
         <v>2022</v>
       </c>
       <c r="C198" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D198">
         <v>224</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4">
       <c r="A199">
         <v>2</v>
       </c>
@@ -3206,13 +3212,13 @@
         <v>2022</v>
       </c>
       <c r="C199" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D199">
         <v>219</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4">
       <c r="A200">
         <v>3</v>
       </c>
@@ -3220,13 +3226,13 @@
         <v>2022</v>
       </c>
       <c r="C200" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D200">
         <v>204</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4">
       <c r="A201">
         <v>4</v>
       </c>
@@ -3234,13 +3240,13 @@
         <v>2022</v>
       </c>
       <c r="C201" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D201">
         <v>173</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4">
       <c r="A202">
         <v>5</v>
       </c>
@@ -3248,13 +3254,13 @@
         <v>2022</v>
       </c>
       <c r="C202" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D202">
         <v>281</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4">
       <c r="A203">
         <v>6</v>
       </c>
@@ -3262,13 +3268,13 @@
         <v>2022</v>
       </c>
       <c r="C203" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D203">
         <v>273</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4">
       <c r="A204">
         <v>7</v>
       </c>
@@ -3276,13 +3282,13 @@
         <v>2022</v>
       </c>
       <c r="C204" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D204">
         <v>287</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4">
       <c r="A205">
         <v>8</v>
       </c>
@@ -3290,13 +3296,13 @@
         <v>2022</v>
       </c>
       <c r="C205" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D205">
         <v>352</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4">
       <c r="A206">
         <v>9</v>
       </c>
@@ -3304,13 +3310,13 @@
         <v>2022</v>
       </c>
       <c r="C206" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D206">
         <v>342</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4">
       <c r="A207">
         <v>10</v>
       </c>
@@ -3318,13 +3324,13 @@
         <v>2022</v>
       </c>
       <c r="C207" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D207">
         <v>101</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4">
       <c r="A208">
         <v>11</v>
       </c>
@@ -3332,13 +3338,13 @@
         <v>2022</v>
       </c>
       <c r="C208" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D208">
         <v>415</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4">
       <c r="A209">
         <v>12</v>
       </c>
@@ -3346,10 +3352,194 @@
         <v>2022</v>
       </c>
       <c r="C209" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D209">
         <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>2023</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2023</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2023</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>2023</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>2023</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>2023</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>2023</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>2024</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>2024</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>2024</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>2024</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>2024</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>2024</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>2024</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>